<commit_message>
v0.7 de SPMP Documentos anexos agregados.
</commit_message>
<xml_diff>
--- a/Proyecto/Primera Entrega/Documentos/(SnoutPoint) - Flujo de caja.xlsx
+++ b/Proyecto/Primera Entrega/Documentos/(SnoutPoint) - Flujo de caja.xlsx
@@ -1121,12 +1121,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1151,15 +1145,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1206,6 +1191,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1513,8 +1513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1535,16 +1535,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="111" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="88"/>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
+      <c r="B1" s="112"/>
+      <c r="C1" s="112"/>
+      <c r="D1" s="112"/>
+      <c r="E1" s="112"/>
     </row>
     <row r="2" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="89" t="s">
+      <c r="A2" s="87" t="s">
         <v>65</v>
       </c>
       <c r="B2" s="86"/>
@@ -1568,7 +1568,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A6" s="90" t="s">
+      <c r="A6" s="88" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1576,13 +1576,13 @@
       <c r="A7" s="84" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="92">
+      <c r="B7" s="90">
         <f>H41</f>
         <v>3640000</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="91" t="s">
+      <c r="A8" s="89" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1592,7 +1592,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A10" s="90" t="s">
+      <c r="A10" s="88" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1600,13 +1600,13 @@
       <c r="A11" s="83" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="93">
+      <c r="B11" s="91">
         <v>10000000</v>
       </c>
-      <c r="C11" s="94" t="s">
+      <c r="C11" s="92" t="s">
         <v>63</v>
       </c>
-      <c r="D11" s="93">
+      <c r="D11" s="91">
         <v>500000</v>
       </c>
       <c r="E11" s="83" t="s">
@@ -1645,36 +1645,36 @@
       <c r="C16" s="10"/>
     </row>
     <row r="17" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A17" s="97" t="s">
+      <c r="A17" s="113" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="98"/>
-      <c r="C17" s="98"/>
-      <c r="D17" s="98"/>
-      <c r="E17" s="98"/>
-      <c r="F17" s="98"/>
-      <c r="G17" s="99"/>
+      <c r="B17" s="114"/>
+      <c r="C17" s="114"/>
+      <c r="D17" s="114"/>
+      <c r="E17" s="114"/>
+      <c r="F17" s="114"/>
+      <c r="G17" s="115"/>
     </row>
     <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="95" t="s">
+      <c r="A18" s="93" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="96">
-        <v>0</v>
-      </c>
-      <c r="C18" s="95">
+      <c r="B18" s="94">
+        <v>0</v>
+      </c>
+      <c r="C18" s="93">
         <v>1</v>
       </c>
-      <c r="D18" s="95">
+      <c r="D18" s="93">
         <v>2</v>
       </c>
-      <c r="E18" s="96">
+      <c r="E18" s="94">
         <v>3</v>
       </c>
-      <c r="F18" s="95">
+      <c r="F18" s="93">
         <v>4</v>
       </c>
-      <c r="G18" s="95">
+      <c r="G18" s="93">
         <v>5</v>
       </c>
       <c r="H18" s="22"/>
@@ -1880,8 +1880,8 @@
         <v>14</v>
       </c>
       <c r="B26" s="17">
-        <f>B55</f>
-        <v>10000000</v>
+        <f>B41</f>
+        <v>11856250</v>
       </c>
       <c r="C26" s="17">
         <f t="shared" ref="C26:G26" si="4">C55</f>
@@ -1910,15 +1910,15 @@
         <v>15</v>
       </c>
       <c r="B27" s="17">
-        <f>B56</f>
-        <v>-10000000</v>
+        <f>-B26</f>
+        <v>-11856250</v>
       </c>
       <c r="C27" s="17">
-        <f t="shared" ref="C27:G27" si="5">C56</f>
-        <v>9500000</v>
+        <f>C56</f>
+        <v>11356250</v>
       </c>
       <c r="D27" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="C27:G27" si="5">D56</f>
         <v>0</v>
       </c>
       <c r="E27" s="17">
@@ -1962,30 +1962,30 @@
       <c r="H28" s="23"/>
     </row>
     <row r="29" spans="1:8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="100" t="s">
+      <c r="A29" s="95" t="s">
         <v>16</v>
       </c>
-      <c r="B29" s="101">
+      <c r="B29" s="96">
         <f>B25+B27-B28</f>
-        <v>-6500000</v>
-      </c>
-      <c r="C29" s="101">
+        <v>-8356250</v>
+      </c>
+      <c r="C29" s="96">
         <f t="shared" ref="C29:G29" si="6">C25+C27-C28</f>
-        <v>9488333.333333334</v>
-      </c>
-      <c r="D29" s="101">
+        <v>11344583.333333334</v>
+      </c>
+      <c r="D29" s="96">
         <f t="shared" si="6"/>
         <v>-11666.666666666664</v>
       </c>
-      <c r="E29" s="101">
+      <c r="E29" s="96">
         <f t="shared" si="6"/>
         <v>-11666.666666666664</v>
       </c>
-      <c r="F29" s="101">
+      <c r="F29" s="96">
         <f t="shared" si="6"/>
         <v>-11666.666666666664</v>
       </c>
-      <c r="G29" s="102">
+      <c r="G29" s="97">
         <f t="shared" si="6"/>
         <v>-421666.66666666669</v>
       </c>
@@ -1993,17 +1993,17 @@
     </row>
     <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="31" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="103" t="s">
+      <c r="A31" s="98" t="s">
         <v>17</v>
       </c>
-      <c r="B31" s="104">
+      <c r="B31" s="99">
         <f>NPV(E31,C29:G29)+B29</f>
-        <v>668852.40676949825</v>
-      </c>
-      <c r="D31" s="105" t="s">
+        <v>240487.02215411328</v>
+      </c>
+      <c r="D31" s="100" t="s">
         <v>56</v>
       </c>
-      <c r="E31" s="106">
+      <c r="E31" s="101">
         <v>0.3</v>
       </c>
     </row>
@@ -2230,23 +2230,23 @@
         <v>220000</v>
       </c>
     </row>
-    <row r="41" spans="1:12" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="B41" s="107">
+      <c r="B41" s="102">
         <f>SUM(B34:B40)</f>
         <v>11856250</v>
       </c>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
-      <c r="E41" s="108">
+      <c r="E41" s="103">
         <f>SUM(E34:E40)</f>
         <v>8800000</v>
       </c>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
-      <c r="H41" s="108">
+      <c r="H41" s="103">
         <f>SUM(H34:H40)</f>
         <v>3640000</v>
       </c>
@@ -2260,7 +2260,7 @@
       <c r="A44" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="G44" s="109" t="s">
+      <c r="G44" s="104" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2283,7 +2283,7 @@
       <c r="F45" s="13">
         <v>4</v>
       </c>
-      <c r="G45" s="110">
+      <c r="G45" s="105">
         <v>5</v>
       </c>
       <c r="H45" s="12">
@@ -2326,7 +2326,7 @@
         <f t="shared" si="8"/>
         <v>2.7777777777777776E-2</v>
       </c>
-      <c r="G46" s="111">
+      <c r="G46" s="106">
         <f t="shared" si="8"/>
         <v>2.7777777777777776E-2</v>
       </c>
@@ -2374,7 +2374,7 @@
         <f t="shared" si="10"/>
         <v>101111.11111111111</v>
       </c>
-      <c r="G47" s="112">
+      <c r="G47" s="107">
         <f t="shared" si="10"/>
         <v>101111.11111111111</v>
       </c>
@@ -2422,7 +2422,7 @@
         <f t="shared" si="12"/>
         <v>505555.55555555556</v>
       </c>
-      <c r="G48" s="112">
+      <c r="G48" s="107">
         <f t="shared" si="12"/>
         <v>606666.66666666663</v>
       </c>
@@ -2470,7 +2470,7 @@
         <f>$B$14-5*F47</f>
         <v>3134444.4444444445</v>
       </c>
-      <c r="G49" s="113">
+      <c r="G49" s="108">
         <f>$B$14-6*G47</f>
         <v>3033333.3333333335</v>
       </c>
@@ -2515,10 +2515,10 @@
       <c r="D51" s="68"/>
       <c r="E51" s="68"/>
       <c r="F51" s="68"/>
-      <c r="G51" s="114" t="s">
+      <c r="G51" s="109" t="s">
         <v>52</v>
       </c>
-      <c r="H51" s="115">
+      <c r="H51" s="110">
         <f>0-0.3*(0-G49)</f>
         <v>910000</v>
       </c>
@@ -2563,7 +2563,8 @@
         <v>40</v>
       </c>
       <c r="B55" s="14">
-        <v>10000000</v>
+        <f>B41</f>
+        <v>11856250</v>
       </c>
       <c r="C55" s="15">
         <v>500000</v>
@@ -2587,11 +2588,11 @@
       </c>
       <c r="B56" s="20">
         <f>-B55</f>
-        <v>-10000000</v>
+        <v>-11856250</v>
       </c>
       <c r="C56" s="21">
         <f>-C55+B55</f>
-        <v>9500000</v>
+        <v>11356250</v>
       </c>
       <c r="D56" s="21">
         <f>-D55+C55</f>

</xml_diff>